<commit_message>
Verificando outliers por produto e alterando tabela Excel
</commit_message>
<xml_diff>
--- a/Relacoes/VendasSazonais/VendasSazonais.xlsx
+++ b/Relacoes/VendasSazonais/VendasSazonais.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ana Clara\Desktop\Consuelo\Relacoes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Consuelo\Relacoes\VendasSazonais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB717A48-E973-4477-BAC0-5DCDC521A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797D93FB-0062-4C7A-8020-782D299225BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="495" windowWidth="19440" windowHeight="11520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VendasSazonais" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,12 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">VendasSazonais!$B$2:$B$1001</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">VendasSazonais!$C$2:$C$1001</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">VendasSazonais!$D$2:$D$1001</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">VendasSazonais!$E$2:$E$1001</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">VendasSazonais!$B$2:$B$1001</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">VendasSazonais!$C$2:$C$1001</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">VendasSazonais!$D$2:$D$1001</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">VendasSazonais!$E$2:$E$1001</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">VendasSazonais!$D$2:$D$1001</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">VendasSazonais!$E$2:$E$1001</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">VendasSazonais!$B$2:$B$1001</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">VendasSazonais!$C$2:$C$1001</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">VendasSazonais!$D$2:$D$1001</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">VendasSazonais!$E$2:$E$1001</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">VendasSazonais!$B$2:$B$1001</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">VendasSazonais!$C$2:$C$1001</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -641,12 +633,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -657,6 +643,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -820,22 +812,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2489,7 +2481,7 @@
   <dimension ref="A1:E1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2502,19 +2494,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -19520,7 +19512,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19528,26 +19521,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402A88C2-D17A-461A-8C85-79CDD9D7F9B4}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A980" workbookViewId="0">
-      <selection activeCell="E1001" sqref="E1001"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -19756,17 +19756,17 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5">
         <v>483</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>368</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="6">
         <v>351</v>
       </c>
     </row>
@@ -19907,19 +19907,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="5">
         <v>309</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>388</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>472</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -20262,17 +20262,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5">
         <v>369</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="5">
         <v>389</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="6">
         <v>324</v>
       </c>
     </row>
@@ -20685,17 +20685,17 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="7">
+      <c r="A69" s="5">
         <v>68</v>
       </c>
-      <c r="B69" s="7">
+      <c r="B69" s="5">
         <v>365</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5">
         <v>390</v>
       </c>
-      <c r="E69" s="8">
+      <c r="E69" s="6">
         <v>311</v>
       </c>
     </row>
@@ -21720,17 +21720,17 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="7">
+      <c r="A130" s="5">
         <v>129</v>
       </c>
-      <c r="B130" s="7">
+      <c r="B130" s="5">
         <v>365</v>
       </c>
-      <c r="C130" s="7"/>
-      <c r="D130" s="7">
+      <c r="C130" s="5"/>
+      <c r="D130" s="5">
         <v>344</v>
       </c>
-      <c r="E130" s="8">
+      <c r="E130" s="6">
         <v>322</v>
       </c>
     </row>
@@ -22092,19 +22092,19 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="7">
+      <c r="A152" s="5">
         <v>151</v>
       </c>
-      <c r="B152" s="7">
+      <c r="B152" s="5">
         <v>366</v>
       </c>
-      <c r="C152" s="7">
+      <c r="C152" s="5">
         <v>388</v>
       </c>
-      <c r="D152" s="7">
+      <c r="D152" s="5">
         <v>469</v>
       </c>
-      <c r="E152" s="8"/>
+      <c r="E152" s="6"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
@@ -23518,15 +23518,15 @@
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="7">
+      <c r="A236" s="5">
         <v>235</v>
       </c>
-      <c r="B236" s="7">
+      <c r="B236" s="5">
         <v>349</v>
       </c>
-      <c r="C236" s="7"/>
-      <c r="D236" s="7"/>
-      <c r="E236" s="8">
+      <c r="C236" s="5"/>
+      <c r="D236" s="5"/>
+      <c r="E236" s="6">
         <v>281</v>
       </c>
     </row>
@@ -24908,17 +24908,17 @@
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="7">
+      <c r="A318" s="5">
         <v>317</v>
       </c>
-      <c r="B318" s="7"/>
-      <c r="C318" s="7">
+      <c r="B318" s="5"/>
+      <c r="C318" s="5">
         <v>341</v>
       </c>
-      <c r="D318" s="7">
+      <c r="D318" s="5">
         <v>310</v>
       </c>
-      <c r="E318" s="8">
+      <c r="E318" s="6">
         <v>317</v>
       </c>
     </row>
@@ -25943,19 +25943,19 @@
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="7">
+      <c r="A379" s="5">
         <v>378</v>
       </c>
-      <c r="B379" s="7">
+      <c r="B379" s="5">
         <v>388</v>
       </c>
-      <c r="C379" s="7">
+      <c r="C379" s="5">
         <v>307</v>
       </c>
-      <c r="D379" s="7">
+      <c r="D379" s="5">
         <v>352</v>
       </c>
-      <c r="E379" s="8"/>
+      <c r="E379" s="6"/>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" s="3">
@@ -26859,17 +26859,17 @@
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A433" s="7">
+      <c r="A433" s="5">
         <v>432</v>
       </c>
-      <c r="B433" s="7">
+      <c r="B433" s="5">
         <v>387</v>
       </c>
-      <c r="C433" s="7">
+      <c r="C433" s="5">
         <v>302</v>
       </c>
-      <c r="D433" s="7"/>
-      <c r="E433" s="8">
+      <c r="D433" s="5"/>
+      <c r="E433" s="6">
         <v>449</v>
       </c>
     </row>
@@ -27112,19 +27112,19 @@
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A448" s="7">
+      <c r="A448" s="5">
         <v>447</v>
       </c>
-      <c r="B448" s="7">
+      <c r="B448" s="5">
         <v>367</v>
       </c>
-      <c r="C448" s="7">
+      <c r="C448" s="5">
         <v>387</v>
       </c>
-      <c r="D448" s="7">
+      <c r="D448" s="5">
         <v>431</v>
       </c>
-      <c r="E448" s="8"/>
+      <c r="E448" s="6"/>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449" s="3">
@@ -27365,17 +27365,17 @@
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A463" s="7">
+      <c r="A463" s="5">
         <v>462</v>
       </c>
-      <c r="B463" s="7"/>
-      <c r="C463" s="7">
+      <c r="B463" s="5"/>
+      <c r="C463" s="5">
         <v>391</v>
       </c>
-      <c r="D463" s="7">
+      <c r="D463" s="5">
         <v>425</v>
       </c>
-      <c r="E463" s="8">
+      <c r="E463" s="6">
         <v>279</v>
       </c>
     </row>
@@ -28706,17 +28706,17 @@
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A542" s="7">
+      <c r="A542" s="5">
         <v>541</v>
       </c>
-      <c r="B542" s="7"/>
-      <c r="C542" s="7">
+      <c r="B542" s="5"/>
+      <c r="C542" s="5">
         <v>357</v>
       </c>
-      <c r="D542" s="7">
+      <c r="D542" s="5">
         <v>305</v>
       </c>
-      <c r="E542" s="8">
+      <c r="E542" s="6">
         <v>334</v>
       </c>
     </row>
@@ -29911,17 +29911,17 @@
       </c>
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A613" s="7">
+      <c r="A613" s="5">
         <v>612</v>
       </c>
-      <c r="B613" s="7"/>
-      <c r="C613" s="7">
+      <c r="B613" s="5"/>
+      <c r="C613" s="5">
         <v>359</v>
       </c>
-      <c r="D613" s="7">
+      <c r="D613" s="5">
         <v>414</v>
       </c>
-      <c r="E613" s="8">
+      <c r="E613" s="6">
         <v>399</v>
       </c>
     </row>
@@ -30317,17 +30317,17 @@
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A637" s="7">
+      <c r="A637" s="5">
         <v>636</v>
       </c>
-      <c r="B637" s="7">
+      <c r="B637" s="5">
         <v>289</v>
       </c>
-      <c r="C637" s="7"/>
-      <c r="D637" s="7">
+      <c r="C637" s="5"/>
+      <c r="D637" s="5">
         <v>417</v>
       </c>
-      <c r="E637" s="8">
+      <c r="E637" s="6">
         <v>417</v>
       </c>
     </row>
@@ -31590,17 +31590,17 @@
       </c>
     </row>
     <row r="712" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A712" s="7">
+      <c r="A712" s="5">
         <v>711</v>
       </c>
-      <c r="B712" s="7">
+      <c r="B712" s="5">
         <v>374</v>
       </c>
-      <c r="C712" s="7"/>
-      <c r="D712" s="7">
+      <c r="C712" s="5"/>
+      <c r="D712" s="5">
         <v>318</v>
       </c>
-      <c r="E712" s="8">
+      <c r="E712" s="6">
         <v>402</v>
       </c>
     </row>
@@ -31894,19 +31894,19 @@
       </c>
     </row>
     <row r="730" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A730" s="7">
+      <c r="A730" s="5">
         <v>729</v>
       </c>
-      <c r="B730" s="7">
+      <c r="B730" s="5">
         <v>322</v>
       </c>
-      <c r="C730" s="7">
+      <c r="C730" s="5">
         <v>382</v>
       </c>
-      <c r="D730" s="7">
+      <c r="D730" s="5">
         <v>391</v>
       </c>
-      <c r="E730" s="8"/>
+      <c r="E730" s="6"/>
     </row>
     <row r="731" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A731" s="3">
@@ -33150,19 +33150,19 @@
       </c>
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A804" s="7">
+      <c r="A804" s="5">
         <v>803</v>
       </c>
-      <c r="B804" s="7">
+      <c r="B804" s="5">
         <v>398</v>
       </c>
-      <c r="C804" s="7">
+      <c r="C804" s="5">
         <v>339</v>
       </c>
-      <c r="D804" s="7">
+      <c r="D804" s="5">
         <v>319</v>
       </c>
-      <c r="E804" s="8"/>
+      <c r="E804" s="6"/>
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="3">
@@ -33811,17 +33811,17 @@
       </c>
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A843" s="7">
+      <c r="A843" s="5">
         <v>842</v>
       </c>
-      <c r="B843" s="7">
+      <c r="B843" s="5">
         <v>391</v>
       </c>
-      <c r="C843" s="7"/>
-      <c r="D843" s="7">
+      <c r="C843" s="5"/>
+      <c r="D843" s="5">
         <v>300</v>
       </c>
-      <c r="E843" s="8">
+      <c r="E843" s="6">
         <v>316</v>
       </c>
     </row>
@@ -36495,17 +36495,17 @@
       </c>
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1001" s="9">
+      <c r="A1001" s="7">
         <v>1000</v>
       </c>
-      <c r="B1001" s="9"/>
-      <c r="C1001" s="9">
+      <c r="B1001" s="7"/>
+      <c r="C1001" s="7">
         <v>269</v>
       </c>
-      <c r="D1001" s="9">
+      <c r="D1001" s="7">
         <v>466</v>
       </c>
-      <c r="E1001" s="10">
+      <c r="E1001" s="8">
         <v>331</v>
       </c>
     </row>

</xml_diff>